<commit_message>
* fix wrong test case * add more format test case
</commit_message>
<xml_diff>
--- a/zss.test/src/test/java/org/zkoss/zss/api/impl/format/TestFile2007-Format.xlsx
+++ b/zss.test/src/test/java/org/zkoss/zss/api/impl/format/TestFile2007-Format.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="90" windowWidth="19395" windowHeight="7785" activeTab="3"/>
+    <workbookView xWindow="600" yWindow="90" windowWidth="19395" windowHeight="7785" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Number" sheetId="1" r:id="rId1"/>
@@ -17,13 +17,14 @@
     <sheet name="Scientific" sheetId="8" r:id="rId8"/>
     <sheet name="Text" sheetId="9" r:id="rId9"/>
     <sheet name="Special" sheetId="10" r:id="rId10"/>
+    <sheet name="Custom" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="121">
   <si>
     <t>Format</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -322,6 +323,129 @@
   </si>
   <si>
     <t>mmmmm-yy;@</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000_ </t>
+  </si>
+  <si>
+    <t>0.00_);[洋紅色](0.00)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.00_);[藍色](0.00)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.00_);[黑色](0.00)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.00_);[青色](0.00)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.00_);[黃色](0.00)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.00_);[白色](0.00)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.00_);[紅色](0.00)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.00_);[綠色](0.00)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mmm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mmmmm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ddd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dddd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yyyy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[h]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[m]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[s]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AM/PM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>am/pm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A/P</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a/p</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mmmm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -329,7 +453,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="70">
+  <numFmts count="99">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="23" formatCode="&quot;US$&quot;#,##0_);\(&quot;US$&quot;#,##0\)"/>
@@ -394,12 +518,41 @@
     <numFmt numFmtId="231" formatCode="h:mm\ AM/PM;@"/>
     <numFmt numFmtId="232" formatCode="e/m/d"/>
     <numFmt numFmtId="233" formatCode="e&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="236" formatCode="yyyy/m/d\ h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="237" formatCode="h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="238" formatCode="d\-mmm;@"/>
-    <numFmt numFmtId="239" formatCode="d\-mmm\-yy;@"/>
-    <numFmt numFmtId="240" formatCode="mmmmm;@"/>
-    <numFmt numFmtId="241" formatCode="mmmmm\-yy;@"/>
+    <numFmt numFmtId="234" formatCode="yyyy/m/d\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="235" formatCode="h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="236" formatCode="d\-mmm;@"/>
+    <numFmt numFmtId="237" formatCode="d\-mmm\-yy;@"/>
+    <numFmt numFmtId="238" formatCode="mmmmm;@"/>
+    <numFmt numFmtId="239" formatCode="mmmmm\-yy;@"/>
+    <numFmt numFmtId="240" formatCode="0.000_ "/>
+    <numFmt numFmtId="241" formatCode="0.00_);[Blue]\(0.00\)"/>
+    <numFmt numFmtId="242" formatCode="0.00_);[Cyan]\(0.00\)"/>
+    <numFmt numFmtId="243" formatCode="0.00_);[Magenta]\(0.00\)"/>
+    <numFmt numFmtId="244" formatCode="0.00_);[Yellow]\(0.00\)"/>
+    <numFmt numFmtId="245" formatCode="0.00_);[Black]\(0.00\)"/>
+    <numFmt numFmtId="246" formatCode="0.00_);[White]\(0.00\)"/>
+    <numFmt numFmtId="247" formatCode="0.00_);[Green]\(0.00\)"/>
+    <numFmt numFmtId="248" formatCode="mm"/>
+    <numFmt numFmtId="249" formatCode="mmm"/>
+    <numFmt numFmtId="250" formatCode="mmmm"/>
+    <numFmt numFmtId="251" formatCode="mmmmm"/>
+    <numFmt numFmtId="252" formatCode="d"/>
+    <numFmt numFmtId="253" formatCode="dd"/>
+    <numFmt numFmtId="254" formatCode="ddd"/>
+    <numFmt numFmtId="255" formatCode="dddd"/>
+    <numFmt numFmtId="256" formatCode="yy"/>
+    <numFmt numFmtId="257" formatCode="yyyy"/>
+    <numFmt numFmtId="258" formatCode="[h]"/>
+    <numFmt numFmtId="259" formatCode="m"/>
+    <numFmt numFmtId="260" formatCode="hh"/>
+    <numFmt numFmtId="261" formatCode="[m]"/>
+    <numFmt numFmtId="262" formatCode="s"/>
+    <numFmt numFmtId="263" formatCode="[s]"/>
+    <numFmt numFmtId="264" formatCode="ss"/>
+    <numFmt numFmtId="265" formatCode="AM/PM"/>
+    <numFmt numFmtId="266" formatCode="am/pm"/>
+    <numFmt numFmtId="267" formatCode="a/p"/>
+    <numFmt numFmtId="268" formatCode="A/P"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -440,7 +593,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -690,6 +843,12 @@
     <xf numFmtId="233" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="234" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="235" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="236" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
@@ -706,6 +865,87 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="241" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="242" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="243" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="244" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="245" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="246" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="247" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="248" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="249" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="250" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="251" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="252" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="253" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="254" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="255" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="256" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="257" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="258" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="259" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="260" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="261" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="262" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="263" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="264" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="265" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="266" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="267" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="268" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1009,10 +1249,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1340,6 +1580,36 @@
         <v>-123456789</v>
       </c>
     </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43">
+        <v>1234.5678</v>
+      </c>
+      <c r="E43" s="7">
+        <v>1234.5678</v>
+      </c>
+      <c r="G43" s="7">
+        <f>C43</f>
+        <v>1234.5678</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45">
+        <v>1234.5678</v>
+      </c>
+      <c r="E45" s="89">
+        <v>1234.5678</v>
+      </c>
+      <c r="G45" s="89">
+        <f>C45</f>
+        <v>1234.5678</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1352,7 +1622,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1487,6 +1757,166 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.75" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="5" max="5" width="25.75" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="7" max="7" width="38.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3">
+        <v>-123456789</v>
+      </c>
+      <c r="E3" s="92">
+        <v>-123456789</v>
+      </c>
+      <c r="G3" s="92">
+        <f>C3</f>
+        <v>-123456789</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5">
+        <v>-123456789</v>
+      </c>
+      <c r="E5" s="90">
+        <v>-123456789</v>
+      </c>
+      <c r="G5" s="90">
+        <f>C5</f>
+        <v>-123456789</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7">
+        <v>-123456789</v>
+      </c>
+      <c r="E7" s="93">
+        <v>-123456789</v>
+      </c>
+      <c r="G7" s="93">
+        <f>C7</f>
+        <v>-123456789</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9">
+        <v>-123456789</v>
+      </c>
+      <c r="E9" s="94">
+        <v>-123456789</v>
+      </c>
+      <c r="G9" s="94">
+        <f>C9</f>
+        <v>-123456789</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11">
+        <v>-123456789</v>
+      </c>
+      <c r="E11" s="91">
+        <v>-123456789</v>
+      </c>
+      <c r="G11" s="91">
+        <f>C11</f>
+        <v>-123456789</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13">
+        <v>-123456789</v>
+      </c>
+      <c r="E13" s="95">
+        <v>-123456789</v>
+      </c>
+      <c r="G13" s="95">
+        <f>C13</f>
+        <v>-123456789</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15">
+        <v>-123456789</v>
+      </c>
+      <c r="E15" s="1">
+        <v>-123456789</v>
+      </c>
+      <c r="G15" s="1">
+        <f>C15</f>
+        <v>-123456789</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17">
+        <v>-123456789</v>
+      </c>
+      <c r="E17" s="96">
+        <v>-123456789</v>
+      </c>
+      <c r="G17" s="96">
+        <f>C17</f>
+        <v>-123456789</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1887,10 +2317,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55:XFD73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2327,6 +2757,156 @@
         <v>41577</v>
       </c>
     </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55" s="22">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="E55" s="97">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="G55" s="97">
+        <f>C55</f>
+        <v>2.4658564814814801</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>100</v>
+      </c>
+      <c r="C57" s="22">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="E57" s="98">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="G57" s="98">
+        <f>C57</f>
+        <v>2.4658564814814801</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>120</v>
+      </c>
+      <c r="C59" s="22">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="E59" s="99">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="G59" s="99">
+        <f>C59</f>
+        <v>2.4658564814814801</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>101</v>
+      </c>
+      <c r="C61" s="22">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="E61" s="100">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="G61" s="100">
+        <f>C61</f>
+        <v>2.4658564814814801</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>102</v>
+      </c>
+      <c r="C63" s="22">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="E63" s="101">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="G63" s="101">
+        <f>C63</f>
+        <v>2.4658564814814801</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>103</v>
+      </c>
+      <c r="C65" s="22">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="E65" s="102">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="G65" s="102">
+        <f>C65</f>
+        <v>2.4658564814814801</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>104</v>
+      </c>
+      <c r="C67" s="22">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="E67" s="103">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="G67" s="103">
+        <f>C67</f>
+        <v>2.4658564814814801</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>105</v>
+      </c>
+      <c r="C69" s="22">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="E69" s="104">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="G69" s="104">
+        <f>C69</f>
+        <v>2.4658564814814801</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>106</v>
+      </c>
+      <c r="C71" s="22">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="E71" s="105">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="G71" s="105">
+        <f>C71</f>
+        <v>2.4658564814814801</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>107</v>
+      </c>
+      <c r="C73" s="22">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="E73" s="106">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="G73" s="106">
+        <f>C73</f>
+        <v>2.4658564814814801</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2336,10 +2916,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E37" sqref="A37:E41"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2661,6 +3241,186 @@
         <v>2.4658564814814814</v>
       </c>
       <c r="G41" s="84">
+        <v>2.4658564814814801</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>108</v>
+      </c>
+      <c r="C43" s="22">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="E43" s="107">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="G43" s="107">
+        <f>C43</f>
+        <v>2.4658564814814801</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45" s="22">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="E45" s="109">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="G45" s="109">
+        <f>C45</f>
+        <v>2.4658564814814801</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>110</v>
+      </c>
+      <c r="C47" s="22">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="E47" s="108">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="G47" s="108">
+        <f>C47</f>
+        <v>2.4658564814814801</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>111</v>
+      </c>
+      <c r="C49" s="22">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="E49" s="110">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="G49" s="110">
+        <f>C49</f>
+        <v>2.4658564814814801</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>112</v>
+      </c>
+      <c r="C51" s="22">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="E51" s="97">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="G51" s="97">
+        <f>C51</f>
+        <v>2.4658564814814801</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>113</v>
+      </c>
+      <c r="C53" s="22">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="E53" s="111">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="G53" s="111">
+        <f>C53</f>
+        <v>2.4658564814814801</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>114</v>
+      </c>
+      <c r="C55" s="22">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="E55" s="112">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="G55" s="112">
+        <f>C55</f>
+        <v>2.4658564814814801</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>115</v>
+      </c>
+      <c r="C57" s="22">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="E57" s="113">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="G57" s="113">
+        <f>C57</f>
+        <v>2.4658564814814801</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>116</v>
+      </c>
+      <c r="C59" s="22">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="E59" s="114">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="G59" s="114">
+        <f>C59</f>
+        <v>2.4658564814814801</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>117</v>
+      </c>
+      <c r="C61" s="22">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="E61" s="115">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="G61" s="115">
+        <f>C61</f>
+        <v>2.4658564814814801</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>118</v>
+      </c>
+      <c r="C63" s="22">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="E63" s="117">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="G63" s="117">
+        <f>C63</f>
+        <v>2.4658564814814801</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>119</v>
+      </c>
+      <c r="C65" s="22">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="E65" s="116">
+        <v>2.4658564814814801</v>
+      </c>
+      <c r="G65" s="116">
+        <f>C65</f>
         <v>2.4658564814814801</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add a special test case for number, #.0,
</commit_message>
<xml_diff>
--- a/zss.test/src/test/java/org/zkoss/zss/api/impl/format/TestFile2007-Format.xlsx
+++ b/zss.test/src/test/java/org/zkoss/zss/api/impl/format/TestFile2007-Format.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="90" windowWidth="19395" windowHeight="7785" activeTab="4"/>
+    <workbookView xWindow="600" yWindow="90" windowWidth="19395" windowHeight="7785"/>
   </bookViews>
   <sheets>
     <sheet name="Number" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="Special" sheetId="10" r:id="rId10"/>
     <sheet name="Custom" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="122">
   <si>
     <t>Format</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -447,125 +447,128 @@
   <si>
     <t>mmmm</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#.0,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="99">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="23" formatCode="&quot;US$&quot;#,##0_);\(&quot;US$&quot;#,##0\)"/>
-    <numFmt numFmtId="24" formatCode="&quot;US$&quot;#,##0_);[Red]\(&quot;US$&quot;#,##0\)"/>
-    <numFmt numFmtId="25" formatCode="&quot;US$&quot;#,##0.00_);\(&quot;US$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="26" formatCode="&quot;US$&quot;#,##0.00_);[Red]\(&quot;US$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="177" formatCode="0.00_);\(0.00\)"/>
-    <numFmt numFmtId="178" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
-    <numFmt numFmtId="179" formatCode="#,##0.00_);\(#,##0.00\)"/>
-    <numFmt numFmtId="180" formatCode="0.00;[Red]0.00"/>
-    <numFmt numFmtId="181" formatCode="0.00_ "/>
-    <numFmt numFmtId="182" formatCode="#,##0.00;[Red]#,##0.00"/>
-    <numFmt numFmtId="183" formatCode="#,##0.00_ "/>
-    <numFmt numFmtId="184" formatCode="0.00_ ;[Red]\-0.00\ "/>
-    <numFmt numFmtId="185" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
-    <numFmt numFmtId="186" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="187" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="188" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="189" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="190" formatCode="&quot;NT$&quot;#,##0.00_);[Red]\(&quot;NT$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="191" formatCode="_-&quot;NT$&quot;* #,##0.00_ ;_-&quot;NT$&quot;* \-#,##0.00\ ;_-&quot;NT$&quot;* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="192" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="193" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
-    <numFmt numFmtId="194" formatCode="m&quot;月&quot;d&quot;日&quot;;@"/>
-    <numFmt numFmtId="195" formatCode="[DBNum1][$-404]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
-    <numFmt numFmtId="196" formatCode="[DBNum1][$-404]m&quot;月&quot;d&quot;日&quot;;@"/>
-    <numFmt numFmtId="197" formatCode="[$-404]aaaa;@"/>
-    <numFmt numFmtId="198" formatCode="[$-404]aaa;@"/>
-    <numFmt numFmtId="199" formatCode="yyyy/m/d;@"/>
-    <numFmt numFmtId="200" formatCode="yyyy/m/d\ h:mm;@"/>
-    <numFmt numFmtId="201" formatCode="[$-409]yyyy/m/d\ h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="202" formatCode="m/d;@"/>
-    <numFmt numFmtId="203" formatCode="m/d/yy;@"/>
-    <numFmt numFmtId="204" formatCode="[$-409]d\-mmm;@"/>
-    <numFmt numFmtId="205" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="206" formatCode="[$-409]mmmmm;@"/>
-    <numFmt numFmtId="207" formatCode="[$-409]mmmmm\-yy;@"/>
-    <numFmt numFmtId="208" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="209" formatCode="h:mm;@"/>
-    <numFmt numFmtId="210" formatCode="[$-409]h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="211" formatCode="h:mm:ss;@"/>
-    <numFmt numFmtId="212" formatCode="[$-409]h:mm:ss\ AM/PM;@"/>
-    <numFmt numFmtId="213" formatCode="h&quot;時&quot;mm&quot;分&quot;;@"/>
-    <numFmt numFmtId="214" formatCode="h&quot;時&quot;mm&quot;分&quot;ss&quot;秒&quot;;@"/>
-    <numFmt numFmtId="215" formatCode="上午/下午h&quot;時&quot;mm&quot;分&quot;;@"/>
-    <numFmt numFmtId="216" formatCode="上午/下午h&quot;時&quot;mm&quot;分&quot;ss&quot;秒&quot;;@"/>
-    <numFmt numFmtId="217" formatCode="#\ ???/???"/>
-    <numFmt numFmtId="218" formatCode="#\ ?/2"/>
-    <numFmt numFmtId="219" formatCode="#\ ?/4"/>
-    <numFmt numFmtId="220" formatCode="#\ ?/8"/>
-    <numFmt numFmtId="221" formatCode="#\ ??/16"/>
-    <numFmt numFmtId="222" formatCode="#\ ?/10"/>
-    <numFmt numFmtId="223" formatCode="#\ ??/100"/>
-    <numFmt numFmtId="224" formatCode="000"/>
-    <numFmt numFmtId="225" formatCode="0000000\-0"/>
-    <numFmt numFmtId="226" formatCode="[&lt;=9999999]###\-####;\(0#\)\ ###\-####"/>
-    <numFmt numFmtId="227" formatCode="[&lt;=99999999]####\-####;\(0#\)\ ####\-####"/>
-    <numFmt numFmtId="228" formatCode="[&gt;99999999]0000\-000\-000;000\-000\-000"/>
-    <numFmt numFmtId="229" formatCode="[DBNum1][$-404]General"/>
-    <numFmt numFmtId="230" formatCode="[DBNum2][$-404]General"/>
-    <numFmt numFmtId="231" formatCode="h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="232" formatCode="e/m/d"/>
-    <numFmt numFmtId="233" formatCode="e&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="234" formatCode="yyyy/m/d\ h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="235" formatCode="h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="236" formatCode="d\-mmm;@"/>
-    <numFmt numFmtId="237" formatCode="d\-mmm\-yy;@"/>
-    <numFmt numFmtId="238" formatCode="mmmmm;@"/>
-    <numFmt numFmtId="239" formatCode="mmmmm\-yy;@"/>
-    <numFmt numFmtId="240" formatCode="0.000_ "/>
-    <numFmt numFmtId="241" formatCode="0.00_);[Blue]\(0.00\)"/>
-    <numFmt numFmtId="242" formatCode="0.00_);[Cyan]\(0.00\)"/>
-    <numFmt numFmtId="243" formatCode="0.00_);[Magenta]\(0.00\)"/>
-    <numFmt numFmtId="244" formatCode="0.00_);[Yellow]\(0.00\)"/>
-    <numFmt numFmtId="245" formatCode="0.00_);[Black]\(0.00\)"/>
-    <numFmt numFmtId="246" formatCode="0.00_);[White]\(0.00\)"/>
-    <numFmt numFmtId="247" formatCode="0.00_);[Green]\(0.00\)"/>
-    <numFmt numFmtId="248" formatCode="mm"/>
-    <numFmt numFmtId="249" formatCode="mmm"/>
-    <numFmt numFmtId="250" formatCode="mmmm"/>
-    <numFmt numFmtId="251" formatCode="mmmmm"/>
-    <numFmt numFmtId="252" formatCode="d"/>
-    <numFmt numFmtId="253" formatCode="dd"/>
-    <numFmt numFmtId="254" formatCode="ddd"/>
-    <numFmt numFmtId="255" formatCode="dddd"/>
-    <numFmt numFmtId="256" formatCode="yy"/>
-    <numFmt numFmtId="257" formatCode="yyyy"/>
-    <numFmt numFmtId="258" formatCode="[h]"/>
-    <numFmt numFmtId="259" formatCode="m"/>
-    <numFmt numFmtId="260" formatCode="hh"/>
-    <numFmt numFmtId="261" formatCode="[m]"/>
-    <numFmt numFmtId="262" formatCode="s"/>
-    <numFmt numFmtId="263" formatCode="[s]"/>
-    <numFmt numFmtId="264" formatCode="ss"/>
-    <numFmt numFmtId="265" formatCode="AM/PM"/>
-    <numFmt numFmtId="266" formatCode="am/pm"/>
-    <numFmt numFmtId="267" formatCode="a/p"/>
-    <numFmt numFmtId="268" formatCode="A/P"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="&quot;US$&quot;#,##0_);\(&quot;US$&quot;#,##0\)"/>
+    <numFmt numFmtId="167" formatCode="&quot;US$&quot;#,##0_);[Red]\(&quot;US$&quot;#,##0\)"/>
+    <numFmt numFmtId="168" formatCode="&quot;US$&quot;#,##0.00_);\(&quot;US$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="169" formatCode="&quot;US$&quot;#,##0.00_);[Red]\(&quot;US$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="170" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="171" formatCode="0.00_);\(0.00\)"/>
+    <numFmt numFmtId="172" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
+    <numFmt numFmtId="173" formatCode="#,##0.00_);\(#,##0.00\)"/>
+    <numFmt numFmtId="174" formatCode="0.00;[Red]0.00"/>
+    <numFmt numFmtId="175" formatCode="0.00_ "/>
+    <numFmt numFmtId="176" formatCode="#,##0.00;[Red]#,##0.00"/>
+    <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
+    <numFmt numFmtId="178" formatCode="0.00_ ;[Red]\-0.00\ "/>
+    <numFmt numFmtId="179" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
+    <numFmt numFmtId="180" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="181" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="182" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="183" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="184" formatCode="&quot;NT$&quot;#,##0.00_);[Red]\(&quot;NT$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="185" formatCode="_-&quot;NT$&quot;* #,##0.00_ ;_-&quot;NT$&quot;* \-#,##0.00\ ;_-&quot;NT$&quot;* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="186" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="187" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
+    <numFmt numFmtId="188" formatCode="m&quot;月&quot;d&quot;日&quot;;@"/>
+    <numFmt numFmtId="189" formatCode="[DBNum1][$-404]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
+    <numFmt numFmtId="190" formatCode="[DBNum1][$-404]m&quot;月&quot;d&quot;日&quot;;@"/>
+    <numFmt numFmtId="191" formatCode="[$-404]aaaa;@"/>
+    <numFmt numFmtId="192" formatCode="[$-404]aaa;@"/>
+    <numFmt numFmtId="193" formatCode="yyyy/m/d;@"/>
+    <numFmt numFmtId="194" formatCode="yyyy/m/d\ h:mm;@"/>
+    <numFmt numFmtId="195" formatCode="[$-409]yyyy/m/d\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="196" formatCode="m/d;@"/>
+    <numFmt numFmtId="197" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="198" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="199" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="200" formatCode="[$-409]mmmmm;@"/>
+    <numFmt numFmtId="201" formatCode="[$-409]mmmmm\-yy;@"/>
+    <numFmt numFmtId="202" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="203" formatCode="h:mm;@"/>
+    <numFmt numFmtId="204" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="205" formatCode="h:mm:ss;@"/>
+    <numFmt numFmtId="206" formatCode="[$-409]h:mm:ss\ AM/PM;@"/>
+    <numFmt numFmtId="207" formatCode="h&quot;時&quot;mm&quot;分&quot;;@"/>
+    <numFmt numFmtId="208" formatCode="h&quot;時&quot;mm&quot;分&quot;ss&quot;秒&quot;;@"/>
+    <numFmt numFmtId="209" formatCode="上午/下午h&quot;時&quot;mm&quot;分&quot;;@"/>
+    <numFmt numFmtId="210" formatCode="上午/下午h&quot;時&quot;mm&quot;分&quot;ss&quot;秒&quot;;@"/>
+    <numFmt numFmtId="211" formatCode="#\ ???/???"/>
+    <numFmt numFmtId="212" formatCode="#\ ?/2"/>
+    <numFmt numFmtId="213" formatCode="#\ ?/4"/>
+    <numFmt numFmtId="214" formatCode="#\ ?/8"/>
+    <numFmt numFmtId="215" formatCode="#\ ??/16"/>
+    <numFmt numFmtId="216" formatCode="#\ ?/10"/>
+    <numFmt numFmtId="217" formatCode="#\ ??/100"/>
+    <numFmt numFmtId="218" formatCode="000"/>
+    <numFmt numFmtId="219" formatCode="0000000\-0"/>
+    <numFmt numFmtId="220" formatCode="[&lt;=9999999]###\-####;\(0#\)\ ###\-####"/>
+    <numFmt numFmtId="221" formatCode="[&lt;=99999999]####\-####;\(0#\)\ ####\-####"/>
+    <numFmt numFmtId="222" formatCode="[&gt;99999999]0000\-000\-000;000\-000\-000"/>
+    <numFmt numFmtId="223" formatCode="[DBNum1][$-404]General"/>
+    <numFmt numFmtId="224" formatCode="[DBNum2][$-404]General"/>
+    <numFmt numFmtId="225" formatCode="h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="226" formatCode="e/m/d"/>
+    <numFmt numFmtId="227" formatCode="e&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="228" formatCode="yyyy/m/d\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="229" formatCode="h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="230" formatCode="d\-mmm;@"/>
+    <numFmt numFmtId="231" formatCode="d\-mmm\-yy;@"/>
+    <numFmt numFmtId="232" formatCode="mmmmm;@"/>
+    <numFmt numFmtId="233" formatCode="mmmmm\-yy;@"/>
+    <numFmt numFmtId="234" formatCode="0.000_ "/>
+    <numFmt numFmtId="235" formatCode="0.00_);[Blue]\(0.00\)"/>
+    <numFmt numFmtId="236" formatCode="0.00_);[Cyan]\(0.00\)"/>
+    <numFmt numFmtId="237" formatCode="0.00_);[Magenta]\(0.00\)"/>
+    <numFmt numFmtId="238" formatCode="0.00_);[Yellow]\(0.00\)"/>
+    <numFmt numFmtId="239" formatCode="0.00_);[Black]\(0.00\)"/>
+    <numFmt numFmtId="240" formatCode="0.00_);[White]\(0.00\)"/>
+    <numFmt numFmtId="241" formatCode="0.00_);[Green]\(0.00\)"/>
+    <numFmt numFmtId="242" formatCode="mm"/>
+    <numFmt numFmtId="243" formatCode="mmm"/>
+    <numFmt numFmtId="244" formatCode="mmmm"/>
+    <numFmt numFmtId="245" formatCode="mmmmm"/>
+    <numFmt numFmtId="246" formatCode="d"/>
+    <numFmt numFmtId="247" formatCode="dd"/>
+    <numFmt numFmtId="248" formatCode="ddd"/>
+    <numFmt numFmtId="249" formatCode="dddd"/>
+    <numFmt numFmtId="250" formatCode="yy"/>
+    <numFmt numFmtId="251" formatCode="yyyy"/>
+    <numFmt numFmtId="252" formatCode="[h]"/>
+    <numFmt numFmtId="253" formatCode="m"/>
+    <numFmt numFmtId="254" formatCode="hh"/>
+    <numFmt numFmtId="255" formatCode="[m]"/>
+    <numFmt numFmtId="256" formatCode="s"/>
+    <numFmt numFmtId="257" formatCode="[s]"/>
+    <numFmt numFmtId="258" formatCode="ss"/>
+    <numFmt numFmtId="259" formatCode="AM/PM"/>
+    <numFmt numFmtId="260" formatCode="a/p"/>
+    <numFmt numFmtId="261" formatCode="A/P"/>
+    <numFmt numFmtId="266" formatCode="#.0,"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -593,16 +596,34 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
@@ -624,12 +645,27 @@
     <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="186" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
@@ -642,27 +678,12 @@
     <xf numFmtId="189" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="190" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="192" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
@@ -720,6 +741,18 @@
     <xf numFmtId="210" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="13" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="211" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
@@ -738,21 +771,15 @@
     <xf numFmtId="216" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="13" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="217" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="218" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
@@ -771,31 +798,7 @@
     <xf numFmtId="223" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="224" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="225" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="226" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="227" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="228" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="229" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="230" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -804,16 +807,16 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="23" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="24" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="25" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="26" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -828,15 +831,33 @@
     <xf numFmtId="48" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="225" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="226" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="227" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="228" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="229" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="230" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="231" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="57" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="232" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
@@ -921,36 +942,21 @@
     <xf numFmtId="259" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="259" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="260" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="261" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="262" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="263" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="264" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="265" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="266" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="267" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="268" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -963,7 +969,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1037,7 +1043,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1072,7 +1077,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1248,14 +1252,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:G5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="29.75" customWidth="1"/>
     <col min="3" max="3" width="24.625" customWidth="1"/>
@@ -1264,7 +1268,7 @@
     <col min="7" max="7" width="40.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1280,7 +1284,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1295,7 +1299,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1310,7 +1314,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1325,7 +1329,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1340,7 +1344,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1355,7 +1359,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1370,7 +1374,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1385,7 +1389,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1400,7 +1404,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1415,7 +1419,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1430,7 +1434,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1445,7 +1449,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -1460,7 +1464,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -1475,7 +1479,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -1490,7 +1494,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -1505,7 +1509,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -1520,7 +1524,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -1535,7 +1539,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -1550,7 +1554,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -1565,7 +1569,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -1580,7 +1584,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -1595,7 +1599,7 @@
         <v>1234.5678</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>90</v>
       </c>
@@ -1608,6 +1612,21 @@
       <c r="G45" s="89">
         <f>C45</f>
         <v>1234.5678</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" t="s">
+        <v>121</v>
+      </c>
+      <c r="C47">
+        <v>12000</v>
+      </c>
+      <c r="E47" s="118">
+        <v>12000</v>
+      </c>
+      <c r="G47" s="118">
+        <f>C47</f>
+        <v>12000</v>
       </c>
     </row>
   </sheetData>
@@ -1618,14 +1637,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="45.375" customWidth="1"/>
     <col min="3" max="3" width="37.875" customWidth="1"/>
@@ -1633,7 +1652,7 @@
     <col min="7" max="7" width="37.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1649,7 +1668,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="60" t="s">
         <v>62</v>
       </c>
@@ -1664,7 +1683,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -1679,7 +1698,7 @@
         <v>156769884</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -1694,7 +1713,7 @@
         <v>21234567</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -1709,7 +1728,7 @@
         <v>212345678</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>66</v>
       </c>
@@ -1724,7 +1743,7 @@
         <v>986956889</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -1739,7 +1758,7 @@
         <v>12345</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>68</v>
       </c>
@@ -1761,14 +1780,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="24.75" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
@@ -1777,7 +1796,7 @@
     <col min="7" max="7" width="38.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1793,7 +1812,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>91</v>
       </c>
@@ -1808,7 +1827,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>92</v>
       </c>
@@ -1823,7 +1842,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>95</v>
       </c>
@@ -1838,7 +1857,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>93</v>
       </c>
@@ -1853,7 +1872,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>94</v>
       </c>
@@ -1868,7 +1887,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>96</v>
       </c>
@@ -1883,7 +1902,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>97</v>
       </c>
@@ -1898,7 +1917,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>98</v>
       </c>
@@ -1921,14 +1940,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="35.25" customWidth="1"/>
     <col min="3" max="3" width="23.625" customWidth="1"/>
@@ -1936,7 +1955,7 @@
     <col min="7" max="7" width="40.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1952,14 +1971,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1974,7 +1993,7 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1989,7 +2008,7 @@
         <v>-1234567890</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -2004,7 +2023,7 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2019,7 +2038,7 @@
         <v>-1234567890</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -2034,7 +2053,7 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -2049,7 +2068,7 @@
         <v>-1234567890</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -2064,7 +2083,7 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -2079,7 +2098,7 @@
         <v>-1234567890</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2094,7 +2113,7 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2109,7 +2128,7 @@
         <v>-1234567890</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -2124,7 +2143,7 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -2139,10 +2158,10 @@
         <v>-1234567890</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="G26" s="22"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" s="60" t="s">
         <v>70</v>
       </c>
@@ -2157,10 +2176,10 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" s="60"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" s="60" t="s">
         <v>71</v>
       </c>
@@ -2175,10 +2194,10 @@
         <v>-1234567890</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" s="60"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" s="60" t="s">
         <v>72</v>
       </c>
@@ -2193,10 +2212,10 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" s="60"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" s="60" t="s">
         <v>73</v>
       </c>
@@ -2218,14 +2237,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="64.25" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
@@ -2233,7 +2252,7 @@
     <col min="7" max="7" width="34.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2249,7 +2268,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -2264,7 +2283,7 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -2279,7 +2298,7 @@
         <v>-1234567890</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -2294,7 +2313,7 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2316,14 +2335,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55:XFD73"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="49.375" customWidth="1"/>
     <col min="3" max="3" width="32.25" customWidth="1"/>
@@ -2331,7 +2350,7 @@
     <col min="7" max="7" width="40.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2347,7 +2366,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -2362,7 +2381,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -2377,7 +2396,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -2392,7 +2411,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -2407,7 +2426,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -2422,12 +2441,12 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="C12" s="22"/>
       <c r="E12" s="22"/>
       <c r="G12" s="22"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -2442,7 +2461,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -2457,7 +2476,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -2472,7 +2491,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -2487,7 +2506,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -2502,12 +2521,12 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="C22" s="22"/>
       <c r="E22" s="22"/>
       <c r="G22" s="22"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -2522,7 +2541,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -2537,7 +2556,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -2552,7 +2571,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -2567,7 +2586,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -2582,7 +2601,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -2597,7 +2616,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -2612,12 +2631,12 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="C36" s="22"/>
       <c r="E36" s="22"/>
       <c r="G36" s="22"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -2632,7 +2651,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7">
       <c r="A39" s="60" t="s">
         <v>78</v>
       </c>
@@ -2647,7 +2666,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7">
       <c r="A41" s="60" t="s">
         <v>79</v>
       </c>
@@ -2662,7 +2681,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7">
       <c r="A43" s="60" t="s">
         <v>80</v>
       </c>
@@ -2677,7 +2696,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7">
       <c r="A45" s="60" t="s">
         <v>81</v>
       </c>
@@ -2692,7 +2711,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>86</v>
       </c>
@@ -2707,7 +2726,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
         <v>87</v>
       </c>
@@ -2722,7 +2741,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
         <v>88</v>
       </c>
@@ -2737,12 +2756,12 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7">
       <c r="C52" s="22"/>
       <c r="E52" s="22"/>
       <c r="G52" s="22"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7">
       <c r="A53" t="s">
         <v>89</v>
       </c>
@@ -2757,7 +2776,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
         <v>99</v>
       </c>
@@ -2772,7 +2791,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7">
       <c r="A57" t="s">
         <v>100</v>
       </c>
@@ -2787,7 +2806,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7">
       <c r="A59" t="s">
         <v>120</v>
       </c>
@@ -2802,7 +2821,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7">
       <c r="A61" t="s">
         <v>101</v>
       </c>
@@ -2817,7 +2836,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7">
       <c r="A63" t="s">
         <v>102</v>
       </c>
@@ -2832,7 +2851,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7">
       <c r="A65" t="s">
         <v>103</v>
       </c>
@@ -2847,7 +2866,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7">
       <c r="A67" t="s">
         <v>104</v>
       </c>
@@ -2862,7 +2881,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7">
       <c r="A69" t="s">
         <v>105</v>
       </c>
@@ -2877,7 +2896,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7">
       <c r="A71" t="s">
         <v>106</v>
       </c>
@@ -2892,7 +2911,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7">
       <c r="A73" t="s">
         <v>107</v>
       </c>
@@ -2915,14 +2934,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="45.375" customWidth="1"/>
     <col min="3" max="3" width="35.875" customWidth="1"/>
@@ -2930,7 +2949,7 @@
     <col min="7" max="7" width="38.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2946,7 +2965,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -2961,7 +2980,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -2976,7 +2995,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -2991,7 +3010,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -3006,7 +3025,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -3021,7 +3040,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -3036,7 +3055,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -3051,7 +3070,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -3066,7 +3085,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -3081,7 +3100,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -3096,7 +3115,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -3111,7 +3130,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" s="60" t="s">
         <v>74</v>
       </c>
@@ -3126,7 +3145,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" s="60" t="s">
         <v>75</v>
       </c>
@@ -3141,7 +3160,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" s="60" t="s">
         <v>76</v>
       </c>
@@ -3156,7 +3175,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>77</v>
       </c>
@@ -3171,7 +3190,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>82</v>
       </c>
@@ -3186,7 +3205,7 @@
         <v>1.4658564814814801</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -3200,7 +3219,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>83</v>
       </c>
@@ -3215,7 +3234,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>84</v>
       </c>
@@ -3230,7 +3249,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -3244,7 +3263,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>108</v>
       </c>
@@ -3259,7 +3278,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>109</v>
       </c>
@@ -3274,7 +3293,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>110</v>
       </c>
@@ -3289,7 +3308,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
         <v>111</v>
       </c>
@@ -3304,7 +3323,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
         <v>112</v>
       </c>
@@ -3319,7 +3338,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7">
       <c r="A53" t="s">
         <v>113</v>
       </c>
@@ -3334,7 +3353,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
         <v>114</v>
       </c>
@@ -3349,7 +3368,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7">
       <c r="A57" t="s">
         <v>115</v>
       </c>
@@ -3364,7 +3383,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7">
       <c r="A59" t="s">
         <v>116</v>
       </c>
@@ -3379,7 +3398,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7">
       <c r="A61" t="s">
         <v>117</v>
       </c>
@@ -3394,7 +3413,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7">
       <c r="A63" t="s">
         <v>118</v>
       </c>
@@ -3409,7 +3428,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7">
       <c r="A65" t="s">
         <v>119</v>
       </c>
@@ -3432,14 +3451,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="33.375" customWidth="1"/>
     <col min="3" max="3" width="32.875" customWidth="1"/>
@@ -3447,7 +3466,7 @@
     <col min="7" max="7" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3463,7 +3482,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="48">
         <v>0</v>
       </c>
@@ -3478,7 +3497,7 @@
         <v>0.98585</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="48">
         <v>0</v>
       </c>
@@ -3493,7 +3512,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="G6" s="22"/>
     </row>
   </sheetData>
@@ -3503,14 +3522,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="39.375" customWidth="1"/>
     <col min="3" max="3" width="27.125" customWidth="1"/>
@@ -3519,7 +3538,7 @@
     <col min="7" max="7" width="36.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3535,7 +3554,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -3550,7 +3569,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -3565,7 +3584,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -3580,7 +3599,7 @@
         <v>0.33085896079999999</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -3595,7 +3614,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -3610,7 +3629,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -3625,7 +3644,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -3640,7 +3659,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -3655,7 +3674,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -3677,14 +3696,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="40.375" customWidth="1"/>
     <col min="3" max="3" width="32.25" customWidth="1"/>
@@ -3693,7 +3712,7 @@
     <col min="7" max="7" width="49.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3709,7 +3728,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="69">
         <v>0</v>
       </c>
@@ -3724,7 +3743,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="68" t="s">
         <v>69</v>
       </c>
@@ -3746,14 +3765,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="28.625" customWidth="1"/>
     <col min="3" max="3" width="38" customWidth="1"/>
@@ -3761,7 +3780,7 @@
     <col min="7" max="7" width="51.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3777,7 +3796,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -3792,7 +3811,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
* add custom format test * update format test file
</commit_message>
<xml_diff>
--- a/zss.test/src/test/java/org/zkoss/zss/api/impl/format/TestFile2007-Format.xlsx
+++ b/zss.test/src/test/java/org/zkoss/zss/api/impl/format/TestFile2007-Format.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="90" windowWidth="19395" windowHeight="7785"/>
+    <workbookView xWindow="600" yWindow="90" windowWidth="19395" windowHeight="7785" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Number" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="Special" sheetId="10" r:id="rId10"/>
     <sheet name="Custom" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="127">
   <si>
     <t>Format</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -449,126 +449,151 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>#.0,</t>
+    <t>$0.00" Surplus";$-0.00" Shortage"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;;&lt;;~;"!"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Text</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># ???/???</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>???.???</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#.000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="99">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="&quot;US$&quot;#,##0_);\(&quot;US$&quot;#,##0\)"/>
-    <numFmt numFmtId="167" formatCode="&quot;US$&quot;#,##0_);[Red]\(&quot;US$&quot;#,##0\)"/>
-    <numFmt numFmtId="168" formatCode="&quot;US$&quot;#,##0.00_);\(&quot;US$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="169" formatCode="&quot;US$&quot;#,##0.00_);[Red]\(&quot;US$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="170" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="171" formatCode="0.00_);\(0.00\)"/>
-    <numFmt numFmtId="172" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
-    <numFmt numFmtId="173" formatCode="#,##0.00_);\(#,##0.00\)"/>
-    <numFmt numFmtId="174" formatCode="0.00;[Red]0.00"/>
-    <numFmt numFmtId="175" formatCode="0.00_ "/>
-    <numFmt numFmtId="176" formatCode="#,##0.00;[Red]#,##0.00"/>
-    <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
-    <numFmt numFmtId="178" formatCode="0.00_ ;[Red]\-0.00\ "/>
-    <numFmt numFmtId="179" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
-    <numFmt numFmtId="180" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="181" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="182" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="183" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="184" formatCode="&quot;NT$&quot;#,##0.00_);[Red]\(&quot;NT$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="185" formatCode="_-&quot;NT$&quot;* #,##0.00_ ;_-&quot;NT$&quot;* \-#,##0.00\ ;_-&quot;NT$&quot;* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="186" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="187" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
-    <numFmt numFmtId="188" formatCode="m&quot;月&quot;d&quot;日&quot;;@"/>
-    <numFmt numFmtId="189" formatCode="[DBNum1][$-404]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
-    <numFmt numFmtId="190" formatCode="[DBNum1][$-404]m&quot;月&quot;d&quot;日&quot;;@"/>
-    <numFmt numFmtId="191" formatCode="[$-404]aaaa;@"/>
-    <numFmt numFmtId="192" formatCode="[$-404]aaa;@"/>
-    <numFmt numFmtId="193" formatCode="yyyy/m/d;@"/>
-    <numFmt numFmtId="194" formatCode="yyyy/m/d\ h:mm;@"/>
-    <numFmt numFmtId="195" formatCode="[$-409]yyyy/m/d\ h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="196" formatCode="m/d;@"/>
-    <numFmt numFmtId="197" formatCode="m/d/yy;@"/>
-    <numFmt numFmtId="198" formatCode="[$-409]d\-mmm;@"/>
-    <numFmt numFmtId="199" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="200" formatCode="[$-409]mmmmm;@"/>
-    <numFmt numFmtId="201" formatCode="[$-409]mmmmm\-yy;@"/>
-    <numFmt numFmtId="202" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="203" formatCode="h:mm;@"/>
-    <numFmt numFmtId="204" formatCode="[$-409]h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="205" formatCode="h:mm:ss;@"/>
-    <numFmt numFmtId="206" formatCode="[$-409]h:mm:ss\ AM/PM;@"/>
-    <numFmt numFmtId="207" formatCode="h&quot;時&quot;mm&quot;分&quot;;@"/>
-    <numFmt numFmtId="208" formatCode="h&quot;時&quot;mm&quot;分&quot;ss&quot;秒&quot;;@"/>
-    <numFmt numFmtId="209" formatCode="上午/下午h&quot;時&quot;mm&quot;分&quot;;@"/>
-    <numFmt numFmtId="210" formatCode="上午/下午h&quot;時&quot;mm&quot;分&quot;ss&quot;秒&quot;;@"/>
-    <numFmt numFmtId="211" formatCode="#\ ???/???"/>
-    <numFmt numFmtId="212" formatCode="#\ ?/2"/>
-    <numFmt numFmtId="213" formatCode="#\ ?/4"/>
-    <numFmt numFmtId="214" formatCode="#\ ?/8"/>
-    <numFmt numFmtId="215" formatCode="#\ ??/16"/>
-    <numFmt numFmtId="216" formatCode="#\ ?/10"/>
-    <numFmt numFmtId="217" formatCode="#\ ??/100"/>
-    <numFmt numFmtId="218" formatCode="000"/>
-    <numFmt numFmtId="219" formatCode="0000000\-0"/>
-    <numFmt numFmtId="220" formatCode="[&lt;=9999999]###\-####;\(0#\)\ ###\-####"/>
-    <numFmt numFmtId="221" formatCode="[&lt;=99999999]####\-####;\(0#\)\ ####\-####"/>
-    <numFmt numFmtId="222" formatCode="[&gt;99999999]0000\-000\-000;000\-000\-000"/>
-    <numFmt numFmtId="223" formatCode="[DBNum1][$-404]General"/>
-    <numFmt numFmtId="224" formatCode="[DBNum2][$-404]General"/>
-    <numFmt numFmtId="225" formatCode="h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="226" formatCode="e/m/d"/>
-    <numFmt numFmtId="227" formatCode="e&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
-    <numFmt numFmtId="228" formatCode="yyyy/m/d\ h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="229" formatCode="h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="230" formatCode="d\-mmm;@"/>
-    <numFmt numFmtId="231" formatCode="d\-mmm\-yy;@"/>
-    <numFmt numFmtId="232" formatCode="mmmmm;@"/>
-    <numFmt numFmtId="233" formatCode="mmmmm\-yy;@"/>
-    <numFmt numFmtId="234" formatCode="0.000_ "/>
-    <numFmt numFmtId="235" formatCode="0.00_);[Blue]\(0.00\)"/>
-    <numFmt numFmtId="236" formatCode="0.00_);[Cyan]\(0.00\)"/>
-    <numFmt numFmtId="237" formatCode="0.00_);[Magenta]\(0.00\)"/>
-    <numFmt numFmtId="238" formatCode="0.00_);[Yellow]\(0.00\)"/>
-    <numFmt numFmtId="239" formatCode="0.00_);[Black]\(0.00\)"/>
-    <numFmt numFmtId="240" formatCode="0.00_);[White]\(0.00\)"/>
-    <numFmt numFmtId="241" formatCode="0.00_);[Green]\(0.00\)"/>
-    <numFmt numFmtId="242" formatCode="mm"/>
-    <numFmt numFmtId="243" formatCode="mmm"/>
-    <numFmt numFmtId="244" formatCode="mmmm"/>
-    <numFmt numFmtId="245" formatCode="mmmmm"/>
-    <numFmt numFmtId="246" formatCode="d"/>
-    <numFmt numFmtId="247" formatCode="dd"/>
-    <numFmt numFmtId="248" formatCode="ddd"/>
-    <numFmt numFmtId="249" formatCode="dddd"/>
-    <numFmt numFmtId="250" formatCode="yy"/>
-    <numFmt numFmtId="251" formatCode="yyyy"/>
-    <numFmt numFmtId="252" formatCode="[h]"/>
-    <numFmt numFmtId="253" formatCode="m"/>
-    <numFmt numFmtId="254" formatCode="hh"/>
-    <numFmt numFmtId="255" formatCode="[m]"/>
-    <numFmt numFmtId="256" formatCode="s"/>
-    <numFmt numFmtId="257" formatCode="[s]"/>
-    <numFmt numFmtId="258" formatCode="ss"/>
-    <numFmt numFmtId="259" formatCode="AM/PM"/>
-    <numFmt numFmtId="260" formatCode="a/p"/>
-    <numFmt numFmtId="261" formatCode="A/P"/>
-    <numFmt numFmtId="266" formatCode="#.0,"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="103">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="23" formatCode="&quot;US$&quot;#,##0_);\(&quot;US$&quot;#,##0\)"/>
+    <numFmt numFmtId="24" formatCode="&quot;US$&quot;#,##0_);[Red]\(&quot;US$&quot;#,##0\)"/>
+    <numFmt numFmtId="25" formatCode="&quot;US$&quot;#,##0.00_);\(&quot;US$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="26" formatCode="&quot;US$&quot;#,##0.00_);[Red]\(&quot;US$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="177" formatCode="0.00_);\(0.00\)"/>
+    <numFmt numFmtId="178" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
+    <numFmt numFmtId="179" formatCode="#,##0.00_);\(#,##0.00\)"/>
+    <numFmt numFmtId="180" formatCode="0.00;[Red]0.00"/>
+    <numFmt numFmtId="181" formatCode="0.00_ "/>
+    <numFmt numFmtId="182" formatCode="#,##0.00;[Red]#,##0.00"/>
+    <numFmt numFmtId="183" formatCode="#,##0.00_ "/>
+    <numFmt numFmtId="184" formatCode="0.00_ ;[Red]\-0.00\ "/>
+    <numFmt numFmtId="185" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
+    <numFmt numFmtId="186" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="187" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="188" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="189" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="190" formatCode="&quot;NT$&quot;#,##0.00_);[Red]\(&quot;NT$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="191" formatCode="_-&quot;NT$&quot;* #,##0.00_ ;_-&quot;NT$&quot;* \-#,##0.00\ ;_-&quot;NT$&quot;* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="192" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="193" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
+    <numFmt numFmtId="194" formatCode="m&quot;月&quot;d&quot;日&quot;;@"/>
+    <numFmt numFmtId="195" formatCode="[DBNum1][$-404]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
+    <numFmt numFmtId="196" formatCode="[DBNum1][$-404]m&quot;月&quot;d&quot;日&quot;;@"/>
+    <numFmt numFmtId="197" formatCode="[$-404]aaaa;@"/>
+    <numFmt numFmtId="198" formatCode="[$-404]aaa;@"/>
+    <numFmt numFmtId="199" formatCode="yyyy/m/d;@"/>
+    <numFmt numFmtId="200" formatCode="yyyy/m/d\ h:mm;@"/>
+    <numFmt numFmtId="201" formatCode="[$-409]yyyy/m/d\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="202" formatCode="m/d;@"/>
+    <numFmt numFmtId="203" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="204" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="205" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="206" formatCode="[$-409]mmmmm;@"/>
+    <numFmt numFmtId="207" formatCode="[$-409]mmmmm\-yy;@"/>
+    <numFmt numFmtId="208" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="209" formatCode="h:mm;@"/>
+    <numFmt numFmtId="210" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="211" formatCode="h:mm:ss;@"/>
+    <numFmt numFmtId="212" formatCode="[$-409]h:mm:ss\ AM/PM;@"/>
+    <numFmt numFmtId="213" formatCode="h&quot;時&quot;mm&quot;分&quot;;@"/>
+    <numFmt numFmtId="214" formatCode="h&quot;時&quot;mm&quot;分&quot;ss&quot;秒&quot;;@"/>
+    <numFmt numFmtId="215" formatCode="上午/下午h&quot;時&quot;mm&quot;分&quot;;@"/>
+    <numFmt numFmtId="216" formatCode="上午/下午h&quot;時&quot;mm&quot;分&quot;ss&quot;秒&quot;;@"/>
+    <numFmt numFmtId="217" formatCode="#\ ???/???"/>
+    <numFmt numFmtId="218" formatCode="#\ ?/2"/>
+    <numFmt numFmtId="219" formatCode="#\ ?/4"/>
+    <numFmt numFmtId="220" formatCode="#\ ?/8"/>
+    <numFmt numFmtId="221" formatCode="#\ ??/16"/>
+    <numFmt numFmtId="222" formatCode="#\ ?/10"/>
+    <numFmt numFmtId="223" formatCode="#\ ??/100"/>
+    <numFmt numFmtId="224" formatCode="000"/>
+    <numFmt numFmtId="225" formatCode="0000000\-0"/>
+    <numFmt numFmtId="226" formatCode="[&lt;=9999999]###\-####;\(0#\)\ ###\-####"/>
+    <numFmt numFmtId="227" formatCode="[&lt;=99999999]####\-####;\(0#\)\ ####\-####"/>
+    <numFmt numFmtId="228" formatCode="[&gt;99999999]0000\-000\-000;000\-000\-000"/>
+    <numFmt numFmtId="229" formatCode="[DBNum1][$-404]General"/>
+    <numFmt numFmtId="230" formatCode="[DBNum2][$-404]General"/>
+    <numFmt numFmtId="231" formatCode="h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="232" formatCode="e/m/d"/>
+    <numFmt numFmtId="233" formatCode="e&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="234" formatCode="yyyy/m/d\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="235" formatCode="h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="236" formatCode="d\-mmm;@"/>
+    <numFmt numFmtId="237" formatCode="d\-mmm\-yy;@"/>
+    <numFmt numFmtId="238" formatCode="mmmmm;@"/>
+    <numFmt numFmtId="239" formatCode="mmmmm\-yy;@"/>
+    <numFmt numFmtId="240" formatCode="0.000_ "/>
+    <numFmt numFmtId="241" formatCode="0.00_);[Blue]\(0.00\)"/>
+    <numFmt numFmtId="242" formatCode="0.00_);[Cyan]\(0.00\)"/>
+    <numFmt numFmtId="243" formatCode="0.00_);[Magenta]\(0.00\)"/>
+    <numFmt numFmtId="244" formatCode="0.00_);[Yellow]\(0.00\)"/>
+    <numFmt numFmtId="245" formatCode="0.00_);[Black]\(0.00\)"/>
+    <numFmt numFmtId="246" formatCode="0.00_);[White]\(0.00\)"/>
+    <numFmt numFmtId="247" formatCode="0.00_);[Green]\(0.00\)"/>
+    <numFmt numFmtId="248" formatCode="mm"/>
+    <numFmt numFmtId="249" formatCode="mmm"/>
+    <numFmt numFmtId="250" formatCode="mmmm"/>
+    <numFmt numFmtId="251" formatCode="mmmmm"/>
+    <numFmt numFmtId="252" formatCode="d"/>
+    <numFmt numFmtId="253" formatCode="dd"/>
+    <numFmt numFmtId="254" formatCode="ddd"/>
+    <numFmt numFmtId="255" formatCode="dddd"/>
+    <numFmt numFmtId="256" formatCode="yy"/>
+    <numFmt numFmtId="257" formatCode="yyyy"/>
+    <numFmt numFmtId="258" formatCode="[h]"/>
+    <numFmt numFmtId="259" formatCode="m"/>
+    <numFmt numFmtId="260" formatCode="hh"/>
+    <numFmt numFmtId="261" formatCode="[m]"/>
+    <numFmt numFmtId="262" formatCode="s"/>
+    <numFmt numFmtId="263" formatCode="[s]"/>
+    <numFmt numFmtId="264" formatCode="ss"/>
+    <numFmt numFmtId="265" formatCode="AM/PM"/>
+    <numFmt numFmtId="266" formatCode="am/pm"/>
+    <numFmt numFmtId="267" formatCode="a/p"/>
+    <numFmt numFmtId="268" formatCode="A/P"/>
+    <numFmt numFmtId="273" formatCode="&quot;$&quot;0.00&quot; Surplus&quot;;&quot;$&quot;\-0.00&quot; Shortage&quot;"/>
+    <numFmt numFmtId="275" formatCode="\&gt;;\&lt;;\~;&quot;!&quot;"/>
+    <numFmt numFmtId="276" formatCode="???.???"/>
+    <numFmt numFmtId="277" formatCode="#.000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -596,34 +621,16 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
@@ -645,19 +652,37 @@
     <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="186" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="188" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="189" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="190" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -666,24 +691,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="188" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="189" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="190" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="192" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
@@ -741,6 +748,24 @@
     <xf numFmtId="210" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="211" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="212" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="213" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="214" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="215" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="216" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
@@ -753,52 +778,52 @@
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="211" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="212" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="213" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="214" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="215" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="216" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="217" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="218" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="219" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="220" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="221" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="222" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="223" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="218" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="219" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="220" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="221" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="222" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="223" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="224" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="225" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="226" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="227" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="228" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="229" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="230" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -807,16 +832,16 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="23" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="24" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="25" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="26" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -831,33 +856,15 @@
     <xf numFmtId="48" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="225" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="226" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="227" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="228" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="229" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="230" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="231" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="57" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="232" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
@@ -942,21 +949,54 @@
     <xf numFmtId="259" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="259" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="260" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="261" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="262" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="263" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="264" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="265" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="266" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="267" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="268" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="273" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="275" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="275" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="276" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="277" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -969,7 +1009,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1043,6 +1083,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1077,6 +1118,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1252,14 +1294,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.75" customWidth="1"/>
     <col min="3" max="3" width="24.625" customWidth="1"/>
@@ -1268,7 +1310,7 @@
     <col min="7" max="7" width="40.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1284,7 +1326,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1299,7 +1341,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1314,7 +1356,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1329,7 +1371,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1344,7 +1386,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1359,7 +1401,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1374,7 +1416,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1389,7 +1431,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1404,7 +1446,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1419,7 +1461,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1434,7 +1476,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1449,7 +1491,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -1464,7 +1506,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -1479,7 +1521,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -1494,7 +1536,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -1509,7 +1551,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -1524,7 +1566,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -1539,7 +1581,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -1554,7 +1596,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -1569,7 +1611,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -1584,7 +1626,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -1599,7 +1641,7 @@
         <v>1234.5678</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>90</v>
       </c>
@@ -1612,21 +1654,6 @@
       <c r="G45" s="89">
         <f>C45</f>
         <v>1234.5678</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" t="s">
-        <v>121</v>
-      </c>
-      <c r="C47">
-        <v>12000</v>
-      </c>
-      <c r="E47" s="118">
-        <v>12000</v>
-      </c>
-      <c r="G47" s="118">
-        <f>C47</f>
-        <v>12000</v>
       </c>
     </row>
   </sheetData>
@@ -1637,14 +1664,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.375" customWidth="1"/>
     <col min="3" max="3" width="37.875" customWidth="1"/>
@@ -1652,7 +1679,7 @@
     <col min="7" max="7" width="37.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1668,7 +1695,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">
         <v>62</v>
       </c>
@@ -1683,7 +1710,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -1698,7 +1725,7 @@
         <v>156769884</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -1713,7 +1740,7 @@
         <v>21234567</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -1728,7 +1755,7 @@
         <v>212345678</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>66</v>
       </c>
@@ -1743,7 +1770,7 @@
         <v>986956889</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -1758,7 +1785,7 @@
         <v>12345</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>68</v>
       </c>
@@ -1780,14 +1807,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.75" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
@@ -1796,7 +1823,7 @@
     <col min="7" max="7" width="38.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1812,7 +1839,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>91</v>
       </c>
@@ -1827,7 +1854,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>92</v>
       </c>
@@ -1842,7 +1869,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>95</v>
       </c>
@@ -1857,7 +1884,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>93</v>
       </c>
@@ -1872,7 +1899,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>94</v>
       </c>
@@ -1887,7 +1914,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>96</v>
       </c>
@@ -1902,7 +1929,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>97</v>
       </c>
@@ -1917,7 +1944,7 @@
         <v>-123456789</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>98</v>
       </c>
@@ -1930,6 +1957,141 @@
       <c r="G17" s="96">
         <f>C17</f>
         <v>-123456789</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19">
+        <v>125.74</v>
+      </c>
+      <c r="E19" s="118">
+        <v>125.74</v>
+      </c>
+      <c r="G19" s="118">
+        <f>C19</f>
+        <v>125.74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21">
+        <v>-125.74</v>
+      </c>
+      <c r="E21" s="118">
+        <v>-125.74</v>
+      </c>
+      <c r="G21" s="118">
+        <f>C21</f>
+        <v>-125.74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="E23" s="119">
+        <v>1</v>
+      </c>
+      <c r="G23" s="119">
+        <f>C23</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="E25" s="119">
+        <v>0</v>
+      </c>
+      <c r="G25" s="119">
+        <f>C25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27">
+        <v>-1</v>
+      </c>
+      <c r="E27" s="119">
+        <v>-1</v>
+      </c>
+      <c r="G27" s="119">
+        <f>C27</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29" s="120" t="s">
+        <v>123</v>
+      </c>
+      <c r="E29" s="121" t="s">
+        <v>123</v>
+      </c>
+      <c r="G29" s="121" t="str">
+        <f>C29</f>
+        <v>Text</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31">
+        <v>5.25</v>
+      </c>
+      <c r="E31" s="52">
+        <v>5.25</v>
+      </c>
+      <c r="G31" s="52">
+        <f>C31</f>
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>125</v>
+      </c>
+      <c r="C33">
+        <v>2.8</v>
+      </c>
+      <c r="E33" s="122">
+        <v>2.8</v>
+      </c>
+      <c r="G33" s="122">
+        <f>C33</f>
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>126</v>
+      </c>
+      <c r="C35">
+        <v>8.9</v>
+      </c>
+      <c r="E35" s="123">
+        <v>8.9</v>
+      </c>
+      <c r="G35" s="123">
+        <f>C35</f>
+        <v>8.9</v>
       </c>
     </row>
   </sheetData>
@@ -1940,14 +2102,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.25" customWidth="1"/>
     <col min="3" max="3" width="23.625" customWidth="1"/>
@@ -1955,7 +2117,7 @@
     <col min="7" max="7" width="40.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1971,14 +2133,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1993,7 +2155,7 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -2008,7 +2170,7 @@
         <v>-1234567890</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -2023,7 +2185,7 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2038,7 +2200,7 @@
         <v>-1234567890</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -2053,7 +2215,7 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -2068,7 +2230,7 @@
         <v>-1234567890</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -2083,7 +2245,7 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -2098,7 +2260,7 @@
         <v>-1234567890</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2113,7 +2275,7 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2128,7 +2290,7 @@
         <v>-1234567890</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -2143,7 +2305,7 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -2158,10 +2320,10 @@
         <v>-1234567890</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G26" s="22"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="60" t="s">
         <v>70</v>
       </c>
@@ -2176,10 +2338,10 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="60"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="60" t="s">
         <v>71</v>
       </c>
@@ -2194,10 +2356,10 @@
         <v>-1234567890</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="60"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="60" t="s">
         <v>72</v>
       </c>
@@ -2212,10 +2374,10 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="60"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="60" t="s">
         <v>73</v>
       </c>
@@ -2237,14 +2399,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="64.25" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
@@ -2252,7 +2414,7 @@
     <col min="7" max="7" width="34.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2268,7 +2430,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -2283,7 +2445,7 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -2298,7 +2460,7 @@
         <v>-1234567890</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -2313,7 +2475,7 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2335,14 +2497,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55:XFD73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.375" customWidth="1"/>
     <col min="3" max="3" width="32.25" customWidth="1"/>
@@ -2350,7 +2512,7 @@
     <col min="7" max="7" width="40.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2366,7 +2528,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -2381,7 +2543,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -2396,7 +2558,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -2411,7 +2573,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -2426,7 +2588,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -2441,12 +2603,12 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C12" s="22"/>
       <c r="E12" s="22"/>
       <c r="G12" s="22"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -2461,7 +2623,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -2476,7 +2638,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -2491,7 +2653,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -2506,7 +2668,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -2521,12 +2683,12 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C22" s="22"/>
       <c r="E22" s="22"/>
       <c r="G22" s="22"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -2541,7 +2703,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -2556,7 +2718,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -2571,7 +2733,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -2586,7 +2748,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -2601,7 +2763,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -2616,7 +2778,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -2631,12 +2793,12 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C36" s="22"/>
       <c r="E36" s="22"/>
       <c r="G36" s="22"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -2651,7 +2813,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="60" t="s">
         <v>78</v>
       </c>
@@ -2666,7 +2828,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="60" t="s">
         <v>79</v>
       </c>
@@ -2681,7 +2843,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="60" t="s">
         <v>80</v>
       </c>
@@ -2696,7 +2858,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="60" t="s">
         <v>81</v>
       </c>
@@ -2711,7 +2873,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>86</v>
       </c>
@@ -2726,7 +2888,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>87</v>
       </c>
@@ -2741,7 +2903,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>88</v>
       </c>
@@ -2756,12 +2918,12 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C52" s="22"/>
       <c r="E52" s="22"/>
       <c r="G52" s="22"/>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>89</v>
       </c>
@@ -2776,7 +2938,7 @@
         <v>41577</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>99</v>
       </c>
@@ -2791,7 +2953,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>100</v>
       </c>
@@ -2806,7 +2968,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>120</v>
       </c>
@@ -2821,7 +2983,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>101</v>
       </c>
@@ -2836,7 +2998,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>102</v>
       </c>
@@ -2851,7 +3013,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>103</v>
       </c>
@@ -2866,7 +3028,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>104</v>
       </c>
@@ -2881,7 +3043,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>105</v>
       </c>
@@ -2896,7 +3058,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>106</v>
       </c>
@@ -2911,7 +3073,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>107</v>
       </c>
@@ -2934,14 +3096,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.375" customWidth="1"/>
     <col min="3" max="3" width="35.875" customWidth="1"/>
@@ -2949,7 +3111,7 @@
     <col min="7" max="7" width="38.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2965,7 +3127,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -2980,7 +3142,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -2995,7 +3157,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -3010,7 +3172,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -3025,7 +3187,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -3040,7 +3202,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -3055,7 +3217,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -3070,7 +3232,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -3085,7 +3247,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -3100,7 +3262,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -3115,7 +3277,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -3130,7 +3292,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="60" t="s">
         <v>74</v>
       </c>
@@ -3145,7 +3307,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="60" t="s">
         <v>75</v>
       </c>
@@ -3160,7 +3322,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="60" t="s">
         <v>76</v>
       </c>
@@ -3175,7 +3337,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>77</v>
       </c>
@@ -3190,7 +3352,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>82</v>
       </c>
@@ -3205,7 +3367,7 @@
         <v>1.4658564814814801</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -3219,7 +3381,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>83</v>
       </c>
@@ -3234,7 +3396,7 @@
         <v>0.46585648148148145</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>84</v>
       </c>
@@ -3249,7 +3411,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -3263,7 +3425,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>108</v>
       </c>
@@ -3278,7 +3440,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>109</v>
       </c>
@@ -3293,7 +3455,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>110</v>
       </c>
@@ -3308,7 +3470,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>111</v>
       </c>
@@ -3323,7 +3485,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>112</v>
       </c>
@@ -3338,7 +3500,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>113</v>
       </c>
@@ -3353,7 +3515,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>114</v>
       </c>
@@ -3368,7 +3530,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>115</v>
       </c>
@@ -3383,7 +3545,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>116</v>
       </c>
@@ -3398,7 +3560,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>117</v>
       </c>
@@ -3413,7 +3575,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>118</v>
       </c>
@@ -3428,7 +3590,7 @@
         <v>2.4658564814814801</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>119</v>
       </c>
@@ -3451,14 +3613,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.375" customWidth="1"/>
     <col min="3" max="3" width="32.875" customWidth="1"/>
@@ -3466,7 +3628,7 @@
     <col min="7" max="7" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3482,7 +3644,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="48">
         <v>0</v>
       </c>
@@ -3497,7 +3659,7 @@
         <v>0.98585</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="48">
         <v>0</v>
       </c>
@@ -3512,7 +3674,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G6" s="22"/>
     </row>
   </sheetData>
@@ -3522,14 +3684,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.375" customWidth="1"/>
     <col min="3" max="3" width="27.125" customWidth="1"/>
@@ -3538,7 +3700,7 @@
     <col min="7" max="7" width="36.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3554,7 +3716,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -3569,7 +3731,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -3584,7 +3746,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -3599,7 +3761,7 @@
         <v>0.33085896079999999</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -3614,7 +3776,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -3629,7 +3791,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -3644,7 +3806,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -3659,7 +3821,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -3674,7 +3836,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -3696,14 +3858,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.375" customWidth="1"/>
     <col min="3" max="3" width="32.25" customWidth="1"/>
@@ -3712,7 +3874,7 @@
     <col min="7" max="7" width="49.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3728,7 +3890,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="69">
         <v>0</v>
       </c>
@@ -3743,7 +3905,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="68" t="s">
         <v>69</v>
       </c>
@@ -3765,14 +3927,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.625" customWidth="1"/>
     <col min="3" max="3" width="38" customWidth="1"/>
@@ -3780,7 +3942,7 @@
     <col min="7" max="7" width="51.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3796,7 +3958,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -3811,7 +3973,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>60</v>
       </c>

</xml_diff>